<commit_message>
Added log messages to state machine to trace steps
</commit_message>
<xml_diff>
--- a/Project2/h50-P2/Steven/P2_Project/Weather/WeatherForcast.xlsx
+++ b/Project2/h50-P2/Steven/P2_Project/Weather/WeatherForcast.xlsx
@@ -37,124 +37,124 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
-    <x:t>Tonight
---
-/74°
-Cloudy
-15%
-WSW 4 mph</x:t>
+    <x:t>Today
+68°
+/59°
+Mostly Sunny
+2%
+NW 12 mph</x:t>
   </x:si>
   <x:si>
     <x:t>Thu 11
-89°
-/74°
-Isolated Thunderstorms
-33%
-W 9 mph</x:t>
+83°
+/61°
+Sunny
+1%
+NNW 9 mph</x:t>
   </x:si>
   <x:si>
     <x:t>Fri 12
-90°
-/74°
-Thunderstorms
-77%
-W 7 mph</x:t>
+85°
+/61°
+Sunny
+0%
+NNW 9 mph</x:t>
   </x:si>
   <x:si>
     <x:t>Sat 13
-88°
-/74°
-Thunderstorms
-72%
+81°
+/61°
+Sunny
+1%
+WNW 8 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sun 14
+79°
+/59°
+Sunny
+1%
+NW 8 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mon 15
+76°
+/58°
+Mostly Sunny
+2%
+WNW 8 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tue 16
+69°
+/58°
+Mostly Cloudy
+4%
 WSW 8 mph</x:t>
   </x:si>
   <x:si>
-    <x:t>Sun 14
-87°
-/73°
-Thunderstorms
-80%
-WNW 7 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon 15
-87°
-/73°
-Thunderstorms
-89%
-NW 7 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue 16
-87°
-/73°
-Thunderstorms
-79%
+    <x:t>Wed 17
+66°
+/56°
+Partly Cloudy
+5%
+SSW 9 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thu 18
+67°
+/55°
+Partly Cloudy
+4%
+WSW 8 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fri 19
+69°
+/56°
+Partly Cloudy
+3%
+NNW 9 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sat 20
+68°
+/57°
+Partly Cloudy
+1%
+NNW 9 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sun 21
+69°
+/58°
+Partly Cloudy
+5%
+NNW 9 mph</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mon 22
+69°
+/57°
+Partly Cloudy
+1%
 NW 8 mph</x:t>
   </x:si>
   <x:si>
-    <x:t>Wed 17
-88°
-/73°
-Thunderstorms
-69%
-NNW 8 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thu 18
-88°
-/74°
-Thunderstorms
-60%
+    <x:t>Tue 23
+68°
+/57°
+Partly Cloudy
+1%
 WNW 8 mph</x:t>
   </x:si>
   <x:si>
-    <x:t>Fri 19
-87°
-/73°
-Thunderstorms
-60%
-WNW 8 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sat 20
-89°
-/73°
-Thunderstorms
-60%
-WNW 8 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun 21
-88°
-/73°
-Thunderstorms
-60%
-WNW 8 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon 22
-88°
-/73°
-Thunderstorms
-60%
-WNW 8 mph</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tue 23
-88°
-/73°
-Thunderstorms
-60%
-WNW 8 mph</x:t>
-  </x:si>
-  <x:si>
     <x:t>Wed 24
-88°
-/73°
-Thunderstorms
-60%
-WNW 8 mph</x:t>
+67°
+/57°
+Mostly Sunny
+1%
+WNW 9 mph</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -197,8 +197,53 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="47">
+  <x:cellStyleXfs count="62">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>